<commit_message>
edited some of the state data
</commit_message>
<xml_diff>
--- a/data/state_election_results/illinois_president.xlsx
+++ b/data/state_election_results/illinois_president.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirhamilton/Desktop/Gov_51/covid_election/data/state_election_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B410CE-F78F-4141-AA5D-010CBE25BF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D2DD2D-6859-4B40-9133-90655491F9F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13360" yWindow="4940" windowWidth="17220" windowHeight="13940" xr2:uid="{BB6E68CF-11ED-9341-8445-CAD7BC7738CB}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>biden.percent</t>
   </si>
   <si>
-    <t>County</t>
-  </si>
-  <si>
     <t>Adams</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>Woodford</t>
+  </si>
+  <si>
+    <t>county</t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -405,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,15 +722,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1BD95E-8E6F-8C47-A76A-A35613DAA690}">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -747,7 +745,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>8569</v>
@@ -764,7 +762,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>1114</v>
@@ -781,7 +779,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>2275</v>
@@ -798,7 +796,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>10372</v>
@@ -815,7 +813,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>485</v>
@@ -832,7 +830,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>6545</v>
@@ -849,7 +847,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>674</v>
@@ -866,7 +864,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>2737</v>
@@ -883,7 +881,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>1615</v>
@@ -900,7 +898,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>56596</v>
@@ -917,7 +915,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
         <v>4286</v>
@@ -934,7 +932,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>1990</v>
@@ -951,7 +949,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
         <v>1129</v>
@@ -968,7 +966,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
         <v>4459</v>
@@ -985,7 +983,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <v>7997</v>
@@ -1002,7 +1000,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
         <v>1714792</v>
@@ -1019,7 +1017,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <v>2198</v>
@@ -1036,7 +1034,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
         <v>1141</v>
@@ -1053,7 +1051,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
         <v>24643</v>
@@ -1070,7 +1068,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2">
         <v>2171</v>
@@ -1087,7 +1085,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2">
         <v>2327</v>
@@ -1104,7 +1102,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2">
         <v>281222</v>
@@ -1121,7 +1119,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2">
         <v>1869</v>
@@ -1138,7 +1136,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>488</v>
@@ -1155,7 +1153,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="2">
         <v>3700</v>
@@ -1172,7 +1170,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="2">
         <v>1815</v>
@@ -1189,7 +1187,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2">
         <v>1691</v>
@@ -1206,7 +1204,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="2">
         <v>4690</v>
@@ -1223,7 +1221,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2">
         <v>6371</v>
@@ -1240,7 +1238,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>621</v>
@@ -1257,7 +1255,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2">
         <v>1349</v>
@@ -1274,7 +1272,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2">
         <v>9445</v>
@@ -1291,7 +1289,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>821</v>
@@ -1308,7 +1306,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2">
         <v>1114</v>
@@ -1325,7 +1323,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>449</v>
@@ -1342,7 +1340,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2">
         <v>1186</v>
@@ -1359,7 +1357,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2">
         <v>9762</v>
@@ -1376,7 +1374,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2">
         <v>2895</v>
@@ -1393,7 +1391,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2">
         <v>11104</v>
@@ -1410,7 +1408,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2">
         <v>1006</v>
@@ -1427,7 +1425,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2">
         <v>4597</v>
@@ -1444,7 +1442,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2">
         <v>2956</v>
@@ -1461,7 +1459,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2">
         <v>5097</v>
@@ -1478,7 +1476,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2">
         <v>1280</v>
@@ -1495,7 +1493,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
         <v>130166</v>
@@ -1512,7 +1510,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2">
         <v>20112</v>
@@ -1529,7 +1527,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2">
         <v>33168</v>
@@ -1546,7 +1544,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" s="2">
         <v>10421</v>
@@ -1563,7 +1561,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2">
         <v>204032</v>
@@ -1580,7 +1578,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2">
         <v>21491</v>
@@ -1597,7 +1595,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" s="2">
         <v>1414</v>
@@ -1614,7 +1612,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" s="2">
         <v>6368</v>
@@ -1631,7 +1629,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54" s="2">
         <v>4568</v>
@@ -1648,7 +1646,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" s="2">
         <v>3769</v>
@@ -1665,7 +1663,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" s="2">
         <v>4973</v>
@@ -1682,7 +1680,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" s="2">
         <v>77208</v>
@@ -1699,7 +1697,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" s="2">
         <v>43719</v>
@@ -1716,7 +1714,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" s="2">
         <v>19633</v>
@@ -1733,7 +1731,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60" s="2">
         <v>7313</v>
@@ -1750,7 +1748,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61" s="2">
         <v>56845</v>
@@ -1767,7 +1765,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62" s="2">
         <v>4396</v>
@@ -1784,7 +1782,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63" s="2">
         <v>2004</v>
@@ -1801,7 +1799,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" s="2">
         <v>1984</v>
@@ -1818,7 +1816,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" s="2">
         <v>1719</v>
@@ -1835,7 +1833,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="2">
         <v>2022</v>
@@ -1852,7 +1850,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67" s="2">
         <v>3212</v>
@@ -1869,7 +1867,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" s="2">
         <v>6489</v>
@@ -1886,7 +1884,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" s="2">
         <v>3889</v>
@@ -1903,7 +1901,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" s="2">
         <v>5020</v>
@@ -1920,7 +1918,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" s="2">
         <v>1645</v>
@@ -1937,7 +1935,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" s="2">
         <v>9300</v>
@@ -1954,7 +1952,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" s="2">
         <v>42600</v>
@@ -1971,7 +1969,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" s="2">
         <v>2609</v>
@@ -1988,7 +1986,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" s="2">
         <v>3302</v>
@@ -2005,7 +2003,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" s="2">
         <v>1458</v>
@@ -2022,7 +2020,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>432</v>
@@ -2039,7 +2037,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>891</v>
@@ -2056,7 +2054,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" s="2">
         <v>1309</v>
@@ -2073,7 +2071,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80" s="2">
         <v>3590</v>
@@ -2090,7 +2088,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81" s="2">
         <v>1824</v>
@@ -2107,7 +2105,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82" s="2">
         <v>36647</v>
@@ -2124,7 +2122,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83" s="2">
         <v>66698</v>
@@ -2141,7 +2139,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B84" s="2">
         <v>2786</v>
@@ -2158,7 +2156,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B85" s="2">
         <v>48756</v>
@@ -2175,7 +2173,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B86" s="2">
         <v>1064</v>
@@ -2192,7 +2190,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>569</v>
@@ -2209,7 +2207,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B88" s="2">
         <v>2488</v>
@@ -2226,7 +2224,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B89">
         <v>814</v>
@@ -2243,7 +2241,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90" s="2">
         <v>8756</v>
@@ -2260,7 +2258,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" s="2">
         <v>24486</v>
@@ -2277,7 +2275,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B92" s="2">
         <v>2575</v>
@@ -2294,7 +2292,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B93" s="2">
         <v>10313</v>
@@ -2311,7 +2309,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B94" s="2">
         <v>1248</v>
@@ -2328,7 +2326,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95" s="2">
         <v>3087</v>
@@ -2345,7 +2343,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B96" s="2">
         <v>1639</v>
@@ -2362,7 +2360,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B97" s="2">
         <v>1185</v>
@@ -2379,7 +2377,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B98" s="2">
         <v>1517</v>
@@ -2396,7 +2394,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B99" s="2">
         <v>12195</v>
@@ -2413,7 +2411,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" s="2">
         <v>182957</v>
@@ -2430,7 +2428,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B101" s="2">
         <v>10107</v>
@@ -2447,7 +2445,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102" s="2">
         <v>64056</v>
@@ -2464,7 +2462,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B103" s="2">
         <v>5976</v>

</xml_diff>